<commit_message>
fix: updated score images,fixed image placement for stimuli, and completed main script to be used in fmri.
</commit_message>
<xml_diff>
--- a/log/sub-t_task-imagerating_log.xlsx
+++ b/log/sub-t_task-imagerating_log.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="199" uniqueCount="68">
   <si>
     <t>Trial</t>
   </si>
@@ -61,6 +61,162 @@
   </si>
   <si>
     <t>R4-4.jpg</t>
+  </si>
+  <si>
+    <t>R8-9.jpg</t>
+  </si>
+  <si>
+    <t>R5-4.jpg</t>
+  </si>
+  <si>
+    <t>R7-9.jpg</t>
+  </si>
+  <si>
+    <t>R4-10.jpg</t>
+  </si>
+  <si>
+    <t>T3-4.jpg</t>
+  </si>
+  <si>
+    <t>T6-9.jpg</t>
+  </si>
+  <si>
+    <t>T7-3.jpg</t>
+  </si>
+  <si>
+    <t>R3-2.jpg</t>
+  </si>
+  <si>
+    <t>T7-8.jpg</t>
+  </si>
+  <si>
+    <t>R8-10.jpg</t>
+  </si>
+  <si>
+    <t>T1-6.jpg</t>
+  </si>
+  <si>
+    <t>R2-1.jpg</t>
+  </si>
+  <si>
+    <t>T6-1.jpg</t>
+  </si>
+  <si>
+    <t>T5-1.jpg</t>
+  </si>
+  <si>
+    <t>T3-3.jpg</t>
+  </si>
+  <si>
+    <t>R1-9.jpg</t>
+  </si>
+  <si>
+    <t>R6-2.jpg</t>
+  </si>
+  <si>
+    <t>R5-2.jpg</t>
+  </si>
+  <si>
+    <t>T5-2.jpg</t>
+  </si>
+  <si>
+    <t>R3-6.jpg</t>
+  </si>
+  <si>
+    <t>R2-2.jpg</t>
+  </si>
+  <si>
+    <t>R2-6.jpg</t>
+  </si>
+  <si>
+    <t>T2-6.jpg</t>
+  </si>
+  <si>
+    <t>R6-8.jpg</t>
+  </si>
+  <si>
+    <t>R6-6.jpg</t>
+  </si>
+  <si>
+    <t>R1-1.jpg</t>
+  </si>
+  <si>
+    <t>R2-8.jpg</t>
+  </si>
+  <si>
+    <t>R5-3.jpg</t>
+  </si>
+  <si>
+    <t>R4-8.jpg</t>
+  </si>
+  <si>
+    <t>T5-8.jpg</t>
+  </si>
+  <si>
+    <t>T1-8.jpg</t>
+  </si>
+  <si>
+    <t>T3-7.jpg</t>
+  </si>
+  <si>
+    <t>T6-3.jpg</t>
+  </si>
+  <si>
+    <t>R3-1.jpg</t>
+  </si>
+  <si>
+    <t>T7-9.jpg</t>
+  </si>
+  <si>
+    <t>T7-5.jpg</t>
+  </si>
+  <si>
+    <t>R5-7.jpg</t>
+  </si>
+  <si>
+    <t>R8-1.jpg</t>
+  </si>
+  <si>
+    <t>T4-5.jpg</t>
+  </si>
+  <si>
+    <t>R8-6.jpg</t>
+  </si>
+  <si>
+    <t>T4-1.jpg</t>
+  </si>
+  <si>
+    <t>R5-5.jpg</t>
+  </si>
+  <si>
+    <t>T6-8.jpg</t>
+  </si>
+  <si>
+    <t>R7-8.jpg</t>
+  </si>
+  <si>
+    <t>R3-7.jpg</t>
+  </si>
+  <si>
+    <t>R4-5.jpg</t>
+  </si>
+  <si>
+    <t>R1-8.jpg</t>
+  </si>
+  <si>
+    <t>T2-1.jpg</t>
+  </si>
+  <si>
+    <t>T1-2.jpg</t>
+  </si>
+  <si>
+    <t>R6-5.jpg</t>
+  </si>
+  <si>
+    <t>T6-2.jpg</t>
+  </si>
+  <si>
+    <t>T4-6.jpg</t>
   </si>
 </sst>
 </file>
@@ -112,10 +268,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.796875" customWidth="true"/>
-    <col min="2" max="2" width="7.86328125" customWidth="true"/>
-    <col min="3" max="3" width="8.73046875" customWidth="true"/>
-    <col min="4" max="4" width="12.06640625" customWidth="true"/>
+    <col min="1" max="1" width="4.5546875" customWidth="true"/>
+    <col min="2" max="2" width="7.6640625" customWidth="true"/>
+    <col min="3" max="3" width="8.77734375" customWidth="true"/>
+    <col min="4" max="4" width="12.21875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -134,87 +290,79 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
+        <v>0</v>
+      </c>
+      <c r="B2" s="0"/>
+      <c r="C2" s="0">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B3" s="0"/>
       <c r="C3" s="0">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D3" s="0">
-        <v>0.462308</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>12</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B4" s="0"/>
       <c r="C4" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D4" s="0">
-        <v>0.415074</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>13</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B5" s="0"/>
       <c r="C5" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="0">
-        <v>0.48148869999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>14</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B6" s="0"/>
       <c r="C6" s="0">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D6" s="0">
-        <v>1.1638158000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>6</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>15</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B7" s="0"/>
       <c r="C7" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D7" s="0">
-        <v>0.71503099999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B8" s="0"/>
       <c r="C8" s="0">
@@ -1066,39 +1214,33 @@
     </row>
     <row r="79">
       <c r="A79" s="0">
-        <v>0</v>
-      </c>
-      <c r="B79" s="0"/>
-      <c r="C79" s="0">
-        <v>0</v>
-      </c>
-      <c r="D79" s="0">
-        <v>0</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C79" s="0"/>
+      <c r="D79" s="0"/>
     </row>
     <row r="80">
       <c r="A80" s="0">
-        <v>0</v>
-      </c>
-      <c r="B80" s="0"/>
-      <c r="C80" s="0">
-        <v>0</v>
-      </c>
-      <c r="D80" s="0">
-        <v>0</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C80" s="0"/>
+      <c r="D80" s="0"/>
     </row>
     <row r="81">
       <c r="A81" s="0">
-        <v>0</v>
-      </c>
-      <c r="B81" s="0"/>
-      <c r="C81" s="0">
-        <v>0</v>
-      </c>
-      <c r="D81" s="0">
-        <v>0</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C81" s="0"/>
+      <c r="D81" s="0"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
fix: complete task and event data
</commit_message>
<xml_diff>
--- a/log/sub-t_task-imagerating_log.xlsx
+++ b/log/sub-t_task-imagerating_log.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="199" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="227" uniqueCount="72">
   <si>
     <t>Trial</t>
   </si>
@@ -217,6 +217,18 @@
   </si>
   <si>
     <t>T4-6.jpg</t>
+  </si>
+  <si>
+    <t>R7-4.jpg</t>
+  </si>
+  <si>
+    <t>T1-7.jpg</t>
+  </si>
+  <si>
+    <t>T4-3.jpg</t>
+  </si>
+  <si>
+    <t>T2-10.jpg</t>
   </si>
 </sst>
 </file>
@@ -269,7 +281,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.5546875" customWidth="true"/>
-    <col min="2" max="2" width="7.6640625" customWidth="true"/>
+    <col min="2" max="2" width="8.5546875" customWidth="true"/>
     <col min="3" max="3" width="8.77734375" customWidth="true"/>
     <col min="4" max="4" width="12.21875" customWidth="true"/>
   </cols>
@@ -290,127 +302,107 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>0</v>
-      </c>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0">
-        <v>0</v>
-      </c>
-      <c r="D2" s="0">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0</v>
-      </c>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0">
-        <v>0</v>
-      </c>
-      <c r="D3" s="0">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0</v>
-      </c>
-      <c r="B4" s="0"/>
-      <c r="C4" s="0">
-        <v>0</v>
-      </c>
-      <c r="D4" s="0">
-        <v>0</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0"/>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0</v>
-      </c>
-      <c r="B5" s="0"/>
-      <c r="C5" s="0">
-        <v>0</v>
-      </c>
-      <c r="D5" s="0">
-        <v>0</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="0"/>
+      <c r="D5" s="0"/>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0</v>
-      </c>
-      <c r="B6" s="0"/>
-      <c r="C6" s="0">
-        <v>0</v>
-      </c>
-      <c r="D6" s="0">
-        <v>0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0"/>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0</v>
-      </c>
-      <c r="B7" s="0"/>
-      <c r="C7" s="0">
-        <v>0</v>
-      </c>
-      <c r="D7" s="0">
-        <v>0</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>0</v>
-      </c>
-      <c r="B8" s="0"/>
-      <c r="C8" s="0">
-        <v>0</v>
-      </c>
-      <c r="D8" s="0">
-        <v>0</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>0</v>
-      </c>
-      <c r="B9" s="0"/>
-      <c r="C9" s="0">
-        <v>0</v>
-      </c>
-      <c r="D9" s="0">
-        <v>0</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="0"/>
+      <c r="D9" s="0"/>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0</v>
-      </c>
-      <c r="B10" s="0"/>
-      <c r="C10" s="0">
-        <v>0</v>
-      </c>
-      <c r="D10" s="0">
-        <v>0</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="0"/>
+      <c r="D10" s="0"/>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>0</v>
-      </c>
-      <c r="B11" s="0"/>
-      <c r="C11" s="0">
-        <v>0</v>
-      </c>
-      <c r="D11" s="0">
-        <v>0</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="0"/>
+      <c r="D11" s="0"/>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="0"/>
       <c r="C12" s="0">
@@ -1214,33 +1206,39 @@
     </row>
     <row r="79">
       <c r="A79" s="0">
-        <v>78</v>
-      </c>
-      <c r="B79" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C79" s="0"/>
-      <c r="D79" s="0"/>
+        <v>0</v>
+      </c>
+      <c r="B79" s="0"/>
+      <c r="C79" s="0">
+        <v>0</v>
+      </c>
+      <c r="D79" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="0">
-        <v>79</v>
-      </c>
-      <c r="B80" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C80" s="0"/>
-      <c r="D80" s="0"/>
+        <v>0</v>
+      </c>
+      <c r="B80" s="0"/>
+      <c r="C80" s="0">
+        <v>0</v>
+      </c>
+      <c r="D80" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="0">
-        <v>80</v>
-      </c>
-      <c r="B81" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C81" s="0"/>
-      <c r="D81" s="0"/>
+        <v>0</v>
+      </c>
+      <c r="B81" s="0"/>
+      <c r="C81" s="0">
+        <v>0</v>
+      </c>
+      <c r="D81" s="0">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>